<commit_message>
Update data given results of differenced body size measurements
</commit_message>
<xml_diff>
--- a/experiment/data/bodySize/Corynactis body size measurements - Amelia.xlsx
+++ b/experiment/data/bodySize/Corynactis body size measurements - Amelia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amelia/github/MHWsim/experiment/data/bodySize/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5861EAC8-131B-F84C-B768-1874861DBBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4C9D5E-9FA9-EB45-B211-25CC011DE4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="500" windowWidth="25400" windowHeight="19280" xr2:uid="{62BD7F3B-A361-7441-8079-A65F3CDFBEBC}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="25400" windowHeight="19280" xr2:uid="{62BD7F3B-A361-7441-8079-A65F3CDFBEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="241">
   <si>
     <t>Sampler</t>
   </si>
@@ -750,11 +750,23 @@
   <si>
     <t>PA130475</t>
   </si>
+  <si>
+    <t>PA200287c</t>
+  </si>
+  <si>
+    <t>PA200288c</t>
+  </si>
+  <si>
+    <t>PA200289c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -812,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -822,6 +834,9 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1136,11 +1151,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D129FA4-925D-E749-8055-D13AB8DECCFA}">
-  <dimension ref="A1:P833"/>
+  <dimension ref="A1:P851"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A803" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K836" sqref="K836"/>
+      <pane ySplit="1" topLeftCell="A814" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M843" sqref="M843"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24300,6 +24315,522 @@
         <v>0.73699999999999999</v>
       </c>
     </row>
+    <row r="834" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A834" t="s">
+        <v>10</v>
+      </c>
+      <c r="B834" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C834" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D834" s="5">
+        <v>9</v>
+      </c>
+      <c r="E834" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F834" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G834" s="5">
+        <v>1</v>
+      </c>
+      <c r="H834" s="5">
+        <v>1</v>
+      </c>
+      <c r="I834" s="5">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="J834" s="5">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="835" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A835" t="s">
+        <v>10</v>
+      </c>
+      <c r="B835" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C835" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D835" s="5">
+        <v>9</v>
+      </c>
+      <c r="E835" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F835" s="5"/>
+      <c r="G835" s="5"/>
+      <c r="H835" s="5">
+        <v>2</v>
+      </c>
+      <c r="I835" s="5">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="J835" s="5">
+        <v>0.435</v>
+      </c>
+    </row>
+    <row r="836" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A836" t="s">
+        <v>10</v>
+      </c>
+      <c r="B836" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C836" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D836" s="5">
+        <v>9</v>
+      </c>
+      <c r="E836" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F836" s="5"/>
+      <c r="G836" s="5"/>
+      <c r="H836" s="5">
+        <v>3</v>
+      </c>
+      <c r="I836" s="5">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="J836" s="5">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="837" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A837" t="s">
+        <v>10</v>
+      </c>
+      <c r="B837" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C837" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D837" s="5">
+        <v>9</v>
+      </c>
+      <c r="E837" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F837" s="5"/>
+      <c r="G837" s="5"/>
+      <c r="H837" s="5">
+        <v>4</v>
+      </c>
+      <c r="I837" s="5">
+        <v>1.077</v>
+      </c>
+      <c r="J837" s="10">
+        <v>0.73299999999999998</v>
+      </c>
+    </row>
+    <row r="838" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A838" t="s">
+        <v>10</v>
+      </c>
+      <c r="B838" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C838" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D838" s="5">
+        <v>9</v>
+      </c>
+      <c r="E838" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F838" s="5"/>
+      <c r="G838" s="5"/>
+      <c r="H838" s="5">
+        <v>5</v>
+      </c>
+      <c r="I838" s="5">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="J838" s="5">
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="839" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A839" t="s">
+        <v>10</v>
+      </c>
+      <c r="B839" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C839" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D839" s="5">
+        <v>9</v>
+      </c>
+      <c r="E839" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F839" s="5"/>
+      <c r="G839" s="7"/>
+      <c r="H839" s="7">
+        <v>6</v>
+      </c>
+      <c r="I839" s="7">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="J839" s="7">
+        <v>0.45900000000000002</v>
+      </c>
+    </row>
+    <row r="840" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A840" t="s">
+        <v>10</v>
+      </c>
+      <c r="B840" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C840" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D840" s="5">
+        <v>9</v>
+      </c>
+      <c r="E840" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F840" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G840" s="7">
+        <v>2</v>
+      </c>
+      <c r="H840" s="7">
+        <v>1</v>
+      </c>
+      <c r="I840" s="11">
+        <v>0.624</v>
+      </c>
+      <c r="J840" s="7">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="841" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A841" t="s">
+        <v>10</v>
+      </c>
+      <c r="B841" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C841" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D841" s="5">
+        <v>9</v>
+      </c>
+      <c r="E841" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F841" s="5"/>
+      <c r="G841" s="7"/>
+      <c r="H841" s="7">
+        <v>2</v>
+      </c>
+      <c r="I841" s="7">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="J841" s="7">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="842" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A842" t="s">
+        <v>10</v>
+      </c>
+      <c r="B842" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C842" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D842" s="5">
+        <v>9</v>
+      </c>
+      <c r="E842" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F842" s="5"/>
+      <c r="G842" s="7"/>
+      <c r="H842" s="7">
+        <v>3</v>
+      </c>
+      <c r="I842" s="11">
+        <v>1.079</v>
+      </c>
+      <c r="J842" s="7">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="843" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A843" t="s">
+        <v>10</v>
+      </c>
+      <c r="B843" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C843" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D843" s="5">
+        <v>9</v>
+      </c>
+      <c r="E843" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F843" s="5"/>
+      <c r="G843" s="7"/>
+      <c r="H843" s="7">
+        <v>4</v>
+      </c>
+      <c r="I843" s="7">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="J843" s="7">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="844" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A844" t="s">
+        <v>10</v>
+      </c>
+      <c r="B844" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C844" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D844" s="5">
+        <v>9</v>
+      </c>
+      <c r="E844" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F844" s="5"/>
+      <c r="G844" s="7"/>
+      <c r="H844" s="7">
+        <v>5</v>
+      </c>
+      <c r="I844" s="11">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="J844" s="7">
+        <v>0.40400000000000003</v>
+      </c>
+    </row>
+    <row r="845" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A845" t="s">
+        <v>10</v>
+      </c>
+      <c r="B845" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C845" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D845" s="5">
+        <v>9</v>
+      </c>
+      <c r="E845" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F845" s="5"/>
+      <c r="G845" s="7"/>
+      <c r="H845" s="7">
+        <v>6</v>
+      </c>
+      <c r="I845" s="7">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="J845" s="7">
+        <v>0.54500000000000004</v>
+      </c>
+    </row>
+    <row r="846" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A846" t="s">
+        <v>10</v>
+      </c>
+      <c r="B846" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C846" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D846" s="5">
+        <v>9</v>
+      </c>
+      <c r="E846" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F846" s="5"/>
+      <c r="G846" s="7"/>
+      <c r="H846" s="7">
+        <v>7</v>
+      </c>
+      <c r="I846" s="11">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="J846" s="7">
+        <v>0.34300000000000003</v>
+      </c>
+    </row>
+    <row r="847" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A847" t="s">
+        <v>10</v>
+      </c>
+      <c r="B847" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C847" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D847" s="5">
+        <v>9</v>
+      </c>
+      <c r="E847" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F847" s="5"/>
+      <c r="G847" s="7"/>
+      <c r="H847" s="7">
+        <v>8</v>
+      </c>
+      <c r="I847" s="7">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="J847" s="7">
+        <v>0.70699999999999996</v>
+      </c>
+    </row>
+    <row r="848" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A848" t="s">
+        <v>10</v>
+      </c>
+      <c r="B848" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C848" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D848" s="5">
+        <v>9</v>
+      </c>
+      <c r="E848" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F848" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G848" s="5">
+        <v>3</v>
+      </c>
+      <c r="H848" s="5">
+        <v>1</v>
+      </c>
+      <c r="I848" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J848" s="5">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="849" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A849" t="s">
+        <v>10</v>
+      </c>
+      <c r="B849" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C849" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D849" s="5">
+        <v>9</v>
+      </c>
+      <c r="E849" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F849" s="5"/>
+      <c r="G849" s="5"/>
+      <c r="H849" s="5">
+        <v>2</v>
+      </c>
+      <c r="I849" s="5">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="J849" s="5">
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="850" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A850" t="s">
+        <v>10</v>
+      </c>
+      <c r="B850" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C850" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D850" s="5">
+        <v>9</v>
+      </c>
+      <c r="E850" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F850" s="5"/>
+      <c r="G850" s="5"/>
+      <c r="H850" s="5">
+        <v>3</v>
+      </c>
+      <c r="I850" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="J850" s="5">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="851" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A851" t="s">
+        <v>10</v>
+      </c>
+      <c r="B851" s="2">
+        <v>45544</v>
+      </c>
+      <c r="C851" s="9">
+        <v>45219</v>
+      </c>
+      <c r="D851" s="5">
+        <v>9</v>
+      </c>
+      <c r="E851" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F851" s="5"/>
+      <c r="G851" s="5"/>
+      <c r="H851" s="5">
+        <v>4</v>
+      </c>
+      <c r="I851" s="5">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="J851" s="5">
+        <v>0.499</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>